<commit_message>
updated data, a bit the scripts too
</commit_message>
<xml_diff>
--- a/data/tables/trajan_tout.xlsx
+++ b/data/tables/trajan_tout.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Networks\TrajanNet\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="344">
   <si>
     <t>Id</t>
   </si>
@@ -826,30 +826,12 @@
     <t>spol8</t>
   </si>
   <si>
-    <t>spol9</t>
-  </si>
-  <si>
     <t>Tribun lacticlave</t>
   </si>
   <si>
-    <t>smil1-1</t>
-  </si>
-  <si>
     <t>Province</t>
   </si>
   <si>
-    <t>Tribun de légion</t>
-  </si>
-  <si>
-    <t>smil1-2</t>
-  </si>
-  <si>
-    <t>Tribun Militaire</t>
-  </si>
-  <si>
-    <t>smil1-3</t>
-  </si>
-  <si>
     <t>smil2</t>
   </si>
   <si>
@@ -1067,12 +1049,24 @@
   </si>
   <si>
     <t>Militaire;Militaire;Politico-militaire;Politico-militaire;Politico-militaire;Politico-militaire</t>
+  </si>
+  <si>
+    <t>smil1</t>
+  </si>
+  <si>
+    <t>Garnison de Rome</t>
+  </si>
+  <si>
+    <t>Equestre</t>
+  </si>
+  <si>
+    <t>cpol7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1813,10 +1807,10 @@
         <v>7</v>
       </c>
       <c r="K4" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="L4" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="M4" t="s">
         <v>24</v>
@@ -1863,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
@@ -1913,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="L6" t="s">
         <v>23</v>
@@ -1963,7 +1957,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -2116,7 +2110,7 @@
         <v>45</v>
       </c>
       <c r="L10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="M10" t="s">
         <v>47</v>
@@ -2163,10 +2157,10 @@
         <v>4</v>
       </c>
       <c r="K11" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="L11" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="M11" t="s">
         <v>47</v>
@@ -2263,10 +2257,10 @@
         <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="L13" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="M13" t="s">
         <v>47</v>
@@ -2313,10 +2307,10 @@
         <v>7</v>
       </c>
       <c r="K14" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="L14" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="M14" t="s">
         <v>47</v>
@@ -2363,10 +2357,10 @@
         <v>3</v>
       </c>
       <c r="K15" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="L15" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="M15" t="s">
         <v>47</v>
@@ -2416,7 +2410,7 @@
         <v>73</v>
       </c>
       <c r="L16" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M16" t="s">
         <v>47</v>
@@ -2463,10 +2457,10 @@
         <v>5</v>
       </c>
       <c r="K17" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="L17" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="M17" t="s">
         <v>47</v>
@@ -2516,7 +2510,7 @@
         <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="M18" t="s">
         <v>47</v>
@@ -2613,10 +2607,10 @@
         <v>7</v>
       </c>
       <c r="K20" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="L20" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="M20" t="s">
         <v>47</v>
@@ -2663,10 +2657,10 @@
         <v>3</v>
       </c>
       <c r="K21" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="L21" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="M21" t="s">
         <v>47</v>
@@ -2713,10 +2707,10 @@
         <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="L22" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="M22" t="s">
         <v>47</v>
@@ -2763,10 +2757,10 @@
         <v>3</v>
       </c>
       <c r="K23" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="L23" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="M23" t="s">
         <v>47</v>
@@ -2863,10 +2857,10 @@
         <v>3</v>
       </c>
       <c r="K25" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="L25" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="M25" t="s">
         <v>47</v>
@@ -3016,7 +3010,7 @@
         <v>115</v>
       </c>
       <c r="L28" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="M28" t="s">
         <v>47</v>
@@ -3066,7 +3060,7 @@
         <v>118</v>
       </c>
       <c r="L29" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M29" t="s">
         <v>47</v>
@@ -3263,10 +3257,10 @@
         <v>6</v>
       </c>
       <c r="K33" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="L33" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="M33" t="s">
         <v>47</v>
@@ -3366,7 +3360,7 @@
         <v>137</v>
       </c>
       <c r="L35" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="M35" t="s">
         <v>47</v>
@@ -3416,7 +3410,7 @@
         <v>141</v>
       </c>
       <c r="L36" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M36" t="s">
         <v>47</v>
@@ -3663,10 +3657,10 @@
         <v>3</v>
       </c>
       <c r="K41" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="L41" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="M41" t="s">
         <v>148</v>
@@ -3866,7 +3860,7 @@
         <v>168</v>
       </c>
       <c r="L45" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="M45" t="s">
         <v>148</v>
@@ -4016,7 +4010,7 @@
         <v>176</v>
       </c>
       <c r="L48" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M48" t="s">
         <v>144</v>
@@ -4066,7 +4060,7 @@
         <v>180</v>
       </c>
       <c r="L49" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="M49" t="s">
         <v>148</v>
@@ -4166,7 +4160,7 @@
         <v>185</v>
       </c>
       <c r="L51" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="M51" t="s">
         <v>144</v>
@@ -4213,7 +4207,7 @@
         <v>2</v>
       </c>
       <c r="K52" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="L52" t="s">
         <v>192</v>
@@ -4266,7 +4260,7 @@
         <v>191</v>
       </c>
       <c r="L53" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="M53" t="s">
         <v>148</v>
@@ -4313,10 +4307,10 @@
         <v>7</v>
       </c>
       <c r="K54" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="L54" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="M54" t="s">
         <v>148</v>
@@ -4363,10 +4357,10 @@
         <v>6</v>
       </c>
       <c r="K55" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="L55" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="M55" t="s">
         <v>148</v>
@@ -4413,10 +4407,10 @@
         <v>2</v>
       </c>
       <c r="K56" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="L56" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M56" t="s">
         <v>144</v>
@@ -4513,10 +4507,10 @@
         <v>6</v>
       </c>
       <c r="K58" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="L58" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="M58" t="s">
         <v>148</v>
@@ -4613,10 +4607,10 @@
         <v>3</v>
       </c>
       <c r="K60" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="L60" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="M60" t="s">
         <v>148</v>
@@ -4713,10 +4707,10 @@
         <v>5</v>
       </c>
       <c r="K62" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="L62" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="M62" t="s">
         <v>148</v>
@@ -4963,7 +4957,7 @@
         <v>2</v>
       </c>
       <c r="K67" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="L67" t="s">
         <v>192</v>
@@ -5042,8 +5036,8 @@
   <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C147" sqref="C147"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5080,7 +5074,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D2" t="s">
         <v>236</v>
@@ -5094,7 +5088,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D3" t="s">
         <v>236</v>
@@ -5108,7 +5102,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D4" t="s">
         <v>236</v>
@@ -5122,7 +5116,7 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D5" t="s">
         <v>236</v>
@@ -5136,7 +5130,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D6" t="s">
         <v>236</v>
@@ -5164,7 +5158,7 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -5495,7 +5489,7 @@
         <v>236</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -6016,7 +6010,7 @@
         <v>26</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>236</v>
@@ -6031,7 +6025,7 @@
         <v>31</v>
       </c>
       <c r="C69" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D69" t="s">
         <v>18</v>
@@ -6048,7 +6042,7 @@
         <v>33</v>
       </c>
       <c r="C70" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D70" t="s">
         <v>236</v>
@@ -6062,7 +6056,7 @@
         <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D71" t="s">
         <v>18</v>
@@ -6076,7 +6070,7 @@
         <v>40</v>
       </c>
       <c r="C72" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D72" t="s">
         <v>18</v>
@@ -6146,7 +6140,7 @@
         <v>31</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>236</v>
@@ -6161,7 +6155,7 @@
         <v>33</v>
       </c>
       <c r="C78" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D78" t="s">
         <v>236</v>
@@ -6175,7 +6169,7 @@
         <v>35</v>
       </c>
       <c r="C79" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D79" t="s">
         <v>241</v>
@@ -6189,7 +6183,7 @@
         <v>37</v>
       </c>
       <c r="C80" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D80" t="s">
         <v>18</v>
@@ -6234,7 +6228,7 @@
         <v>64</v>
       </c>
       <c r="C83" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D83" t="s">
         <v>236</v>
@@ -6290,7 +6284,7 @@
         <v>88</v>
       </c>
       <c r="C87" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D87" t="s">
         <v>236</v>
@@ -6408,7 +6402,7 @@
         <v>236</v>
       </c>
       <c r="E95" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -6439,7 +6433,7 @@
         <v>236</v>
       </c>
       <c r="E97" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -6607,7 +6601,7 @@
         <v>33</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D109" s="10" t="s">
         <v>236</v>
@@ -6622,7 +6616,7 @@
         <v>35</v>
       </c>
       <c r="C110" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D110" t="s">
         <v>236</v>
@@ -6636,7 +6630,7 @@
         <v>37</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D111" s="23" t="s">
         <v>18</v>
@@ -6651,7 +6645,7 @@
         <v>40</v>
       </c>
       <c r="C112" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D112" t="s">
         <v>236</v>
@@ -6665,7 +6659,7 @@
         <v>35</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>236</v>
@@ -6680,7 +6674,7 @@
         <v>37</v>
       </c>
       <c r="C114" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D114" t="s">
         <v>18</v>
@@ -6694,7 +6688,7 @@
         <v>40</v>
       </c>
       <c r="C115" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D115" t="s">
         <v>236</v>
@@ -6708,7 +6702,7 @@
         <v>37</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D116" s="10" t="s">
         <v>18</v>
@@ -6723,7 +6717,7 @@
         <v>40</v>
       </c>
       <c r="C117" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D117" t="s">
         <v>18</v>
@@ -6754,7 +6748,7 @@
         <v>40</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D119" s="10" t="s">
         <v>18</v>
@@ -7441,7 +7435,7 @@
         <v>221</v>
       </c>
       <c r="C166" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D166" t="s">
         <v>236</v>
@@ -7467,7 +7461,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7647,7 +7641,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>254</v>
@@ -7662,32 +7656,32 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>254</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>265</v>
+        <v>340</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>266</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
         <v>254</v>
@@ -7699,15 +7693,15 @@
         <v>267</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
         <v>254</v>
@@ -7716,110 +7710,110 @@
         <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>341</v>
       </c>
       <c r="B13" t="s">
-        <v>254</v>
+        <v>342</v>
       </c>
       <c r="C13" t="s">
         <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>230</v>
       </c>
       <c r="D14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>271</v>
       </c>
       <c r="B15" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>230</v>
       </c>
       <c r="D15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C16" t="s">
         <v>230</v>
       </c>
       <c r="D16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>277</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C17" t="s">
         <v>230</v>
       </c>
       <c r="D17" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
         <v>262</v>
@@ -7827,39 +7821,39 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C18" t="s">
         <v>230</v>
       </c>
       <c r="D18" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>262</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C19" t="s">
         <v>230</v>
       </c>
       <c r="D19" t="s">
-        <v>280</v>
+        <v>343</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
         <v>262</v>
@@ -7867,161 +7861,121 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C20" t="s">
-        <v>230</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>212</v>
       </c>
       <c r="B21" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C21" t="s">
-        <v>230</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>279</v>
       </c>
       <c r="B22" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C22" t="s">
         <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>212</v>
+        <v>281</v>
       </c>
       <c r="B23" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C23" t="s">
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B24" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B25" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>289</v>
-      </c>
-      <c r="B26" t="s">
-        <v>275</v>
-      </c>
-      <c r="C26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>290</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>291</v>
-      </c>
-      <c r="B27" t="s">
-        <v>275</v>
-      </c>
-      <c r="C27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" t="s">
-        <v>292</v>
-      </c>
-      <c r="E27">
-        <v>6</v>
-      </c>
-      <c r="F27" t="s">
         <v>262</v>
       </c>
     </row>

</xml_diff>

<commit_message>
many small adjustments, including french text in plots
</commit_message>
<xml_diff>
--- a/data/tables/trajan_tout.xlsx
+++ b/data/tables/trajan_tout.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Eclipse\workspaces\Networks\TrajanNet\data\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Networks\TrajanNet\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5630" windowHeight="1020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5625" windowHeight="1020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="attributs" sheetId="1" r:id="rId1"/>
@@ -1066,7 +1066,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1605,34 +1605,34 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.453125"/>
-    <col min="3" max="3" width="63.7265625" customWidth="1"/>
-    <col min="4" max="4" width="31.7265625" customWidth="1"/>
-    <col min="5" max="5" width="45.54296875" customWidth="1"/>
-    <col min="6" max="6" width="30.81640625" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" customWidth="1"/>
-    <col min="8" max="8" width="55.54296875" customWidth="1"/>
-    <col min="9" max="9" width="29.54296875" customWidth="1"/>
-    <col min="10" max="10" width="18.81640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="58.81640625" customWidth="1"/>
-    <col min="12" max="12" width="53.7265625" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="63.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="55.5703125" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="58.85546875" customWidth="1"/>
+    <col min="12" max="12" width="53.7109375" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="16.1796875" customWidth="1"/>
-    <col min="15" max="15" width="21.1796875" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" customWidth="1"/>
-    <col min="17" max="17" width="27.81640625" customWidth="1"/>
-    <col min="18" max="1025" width="11.453125"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="27.85546875" customWidth="1"/>
+    <col min="18" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>16</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>152</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>157</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>162</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>165</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>171</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>176</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>180</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>185</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>188</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>192</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>194</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>196</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>198</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>201</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>203</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>205</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>207</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>209</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>212</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>216</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>220</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>223</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>225</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>227</v>
       </c>
@@ -5043,20 +5043,20 @@
   <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="1025" width="11.453125"/>
+    <col min="6" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>230</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -5967,7 +5967,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>19</v>
       </c>
@@ -6024,7 +6024,7 @@
       </c>
       <c r="E68" s="10"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>26</v>
       </c>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="E77" s="10"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>26</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -6196,7 +6196,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>26</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>26</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>26</v>
       </c>
@@ -6339,7 +6339,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>26</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>26</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>26</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>26</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>26</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>26</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>26</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>26</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>26</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>26</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>26</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>26</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>26</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>26</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>26</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
         <v>31</v>
       </c>
@@ -6615,7 +6615,7 @@
       </c>
       <c r="E109" s="10"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>31</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="19" t="s">
         <v>31</v>
       </c>
@@ -6644,7 +6644,7 @@
       </c>
       <c r="E111" s="19"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>31</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>33</v>
       </c>
@@ -6673,7 +6673,7 @@
       </c>
       <c r="E113" s="10"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>33</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>33</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
         <v>35</v>
       </c>
@@ -6716,7 +6716,7 @@
       </c>
       <c r="E116" s="10"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>35</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="19" t="s">
         <v>35</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="s">
         <v>37</v>
       </c>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="E119" s="10"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>37</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
         <v>42</v>
       </c>
@@ -6791,7 +6791,7 @@
       </c>
       <c r="E121" s="10"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>42</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>42</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="10" t="s">
         <v>53</v>
       </c>
@@ -6848,7 +6848,7 @@
       </c>
       <c r="E125" s="10"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>53</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
         <v>58</v>
       </c>
@@ -6877,7 +6877,7 @@
       </c>
       <c r="E127" s="10"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>58</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>58</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>58</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>58</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>58</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>64</v>
       </c>
@@ -6962,7 +6962,7 @@
       </c>
       <c r="E133" s="10"/>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>70</v>
       </c>
@@ -6977,7 +6977,7 @@
       </c>
       <c r="E134" s="10"/>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>78</v>
       </c>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="E135" s="10"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>78</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>78</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>81</v>
       </c>
@@ -7035,7 +7035,7 @@
       </c>
       <c r="E138" s="10"/>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>81</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>81</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="10" t="s">
         <v>88</v>
       </c>
@@ -7078,7 +7078,7 @@
       </c>
       <c r="E141" s="10"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>88</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>88</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="20" t="s">
         <v>88</v>
       </c>
@@ -7121,7 +7121,7 @@
       </c>
       <c r="E144" s="20"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="19" t="s">
         <v>92</v>
       </c>
@@ -7136,7 +7136,7 @@
       </c>
       <c r="E145" s="19"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
         <v>99</v>
       </c>
@@ -7151,7 +7151,7 @@
       </c>
       <c r="E146" s="10"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>99</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>99</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="10" t="s">
         <v>102</v>
       </c>
@@ -7194,7 +7194,7 @@
       </c>
       <c r="E149" s="10"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="10" t="s">
         <v>104</v>
       </c>
@@ -7209,7 +7209,7 @@
       </c>
       <c r="E150" s="10"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="10" t="s">
         <v>107</v>
       </c>
@@ -7224,7 +7224,7 @@
       </c>
       <c r="E151" s="10"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="19" t="s">
         <v>107</v>
       </c>
@@ -7239,7 +7239,7 @@
       </c>
       <c r="E152" s="19"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="19" t="s">
         <v>107</v>
       </c>
@@ -7254,7 +7254,7 @@
       </c>
       <c r="E153" s="19"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="19" t="s">
         <v>107</v>
       </c>
@@ -7269,7 +7269,7 @@
       </c>
       <c r="E154" s="19"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="19" t="s">
         <v>107</v>
       </c>
@@ -7284,7 +7284,7 @@
       </c>
       <c r="E155" s="19"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="19" t="s">
         <v>107</v>
       </c>
@@ -7299,7 +7299,7 @@
       </c>
       <c r="E156" s="19"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="19" t="s">
         <v>107</v>
       </c>
@@ -7314,7 +7314,7 @@
       </c>
       <c r="E157" s="19"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="19" t="s">
         <v>107</v>
       </c>
@@ -7329,7 +7329,7 @@
       </c>
       <c r="E158" s="19"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="19" t="s">
         <v>107</v>
       </c>
@@ -7344,7 +7344,7 @@
       </c>
       <c r="E159" s="19"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="19" t="s">
         <v>107</v>
       </c>
@@ -7359,7 +7359,7 @@
       </c>
       <c r="E160" s="19"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="19" t="s">
         <v>107</v>
       </c>
@@ -7374,7 +7374,7 @@
       </c>
       <c r="E161" s="19"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="10" t="s">
         <v>110</v>
       </c>
@@ -7389,7 +7389,7 @@
       </c>
       <c r="E162" s="10"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="10" t="s">
         <v>115</v>
       </c>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="E163" s="10"/>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="10" t="s">
         <v>118</v>
       </c>
@@ -7419,7 +7419,7 @@
       </c>
       <c r="E164" s="10"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="10" t="s">
         <v>162</v>
       </c>
@@ -7434,7 +7434,7 @@
       </c>
       <c r="E165" s="10"/>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>162</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
       <c r="B167" s="10"/>
       <c r="C167" s="10"/>
@@ -7472,21 +7472,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
-    <col min="7" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>247</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>218</v>
       </c>
@@ -7566,7 +7566,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>264</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>340</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>341</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>229</v>
       </c>
       <c r="D13" t="s">
         <v>269</v>
@@ -7746,7 +7746,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>270</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -7846,7 +7846,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -7886,7 +7886,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>211</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>278</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>280</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>282</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>284</v>
       </c>

</xml_diff>

<commit_message>
now handling short character names
</commit_message>
<xml_diff>
--- a/data/tables/trajan_tout.xlsx
+++ b/data/tables/trajan_tout.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="400">
   <si>
     <t>Id</t>
   </si>
@@ -1189,15 +1189,9 @@
     <t>Santra</t>
   </si>
   <si>
-    <t>Minicius Natalis</t>
-  </si>
-  <si>
     <t>Pompeius</t>
   </si>
   <si>
-    <t>Publius Maximus</t>
-  </si>
-  <si>
     <t>Valerius</t>
   </si>
   <si>
@@ -1213,10 +1207,28 @@
     <t>Scaurianus</t>
   </si>
   <si>
-    <t>Vibius Maximus</t>
-  </si>
-  <si>
     <t>Sextus Erucius Clarus</t>
+  </si>
+  <si>
+    <t>Catilius</t>
+  </si>
+  <si>
+    <t>Haterius</t>
+  </si>
+  <si>
+    <t>Natalis</t>
+  </si>
+  <si>
+    <t>Septicius</t>
+  </si>
+  <si>
+    <t>Sosius</t>
+  </si>
+  <si>
+    <t>Publius</t>
+  </si>
+  <si>
+    <t>Vibius</t>
   </si>
 </sst>
 </file>
@@ -1761,10 +1773,10 @@
   <dimension ref="A1:Q68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2487,7 +2499,7 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>346</v>
+        <v>393</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -4074,7 +4086,7 @@
         <v>155</v>
       </c>
       <c r="B44" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C44" t="s">
         <v>374</v>
@@ -4289,7 +4301,7 @@
         <v>166</v>
       </c>
       <c r="C48" t="s">
-        <v>378</v>
+        <v>394</v>
       </c>
       <c r="D48" t="s">
         <v>66</v>
@@ -4819,7 +4831,7 @@
         <v>193</v>
       </c>
       <c r="C58" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D58" t="s">
         <v>103</v>
@@ -4872,7 +4884,7 @@
         <v>195</v>
       </c>
       <c r="C59" t="s">
-        <v>195</v>
+        <v>397</v>
       </c>
       <c r="D59" t="s">
         <v>16</v>
@@ -4925,7 +4937,7 @@
         <v>197</v>
       </c>
       <c r="C60" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D60" t="s">
         <v>66</v>
@@ -4978,7 +4990,7 @@
         <v>199</v>
       </c>
       <c r="C61" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="D61" t="s">
         <v>152</v>
@@ -5031,7 +5043,7 @@
         <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D62" t="s">
         <v>26</v>
@@ -5084,7 +5096,7 @@
         <v>204</v>
       </c>
       <c r="C63" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D63" t="s">
         <v>95</v>
@@ -5137,7 +5149,7 @@
         <v>208</v>
       </c>
       <c r="C64" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D64" t="s">
         <v>209</v>
@@ -5190,7 +5202,7 @@
         <v>212</v>
       </c>
       <c r="C65" t="s">
-        <v>374</v>
+        <v>396</v>
       </c>
       <c r="D65" t="s">
         <v>16</v>
@@ -5243,7 +5255,7 @@
         <v>215</v>
       </c>
       <c r="C66" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D66" t="s">
         <v>16</v>
@@ -5296,7 +5308,7 @@
         <v>217</v>
       </c>
       <c r="C67" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D67" t="s">
         <v>66</v>
@@ -5349,7 +5361,7 @@
         <v>219</v>
       </c>
       <c r="C68" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="D68" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
started dealing with sequences
</commit_message>
<xml_diff>
--- a/data/tables/trajan_tout.xlsx
+++ b/data/tables/trajan_tout.xlsx
@@ -15,11 +15,12 @@
     <sheet name="attributs" sheetId="1" r:id="rId1"/>
     <sheet name="relations" sheetId="2" r:id="rId2"/>
     <sheet name="postes" sheetId="3" r:id="rId3"/>
+    <sheet name="carrieres" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">relations!$A$1:$E$166</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="444">
   <si>
     <t>Id</t>
   </si>
@@ -1229,13 +1230,145 @@
   </si>
   <si>
     <t>Vibius</t>
+  </si>
+  <si>
+    <t>Carriere</t>
+  </si>
+  <si>
+    <t>Type de carrière</t>
+  </si>
+  <si>
+    <t>Sequence type</t>
+  </si>
+  <si>
+    <t>Sénateur</t>
+  </si>
+  <si>
+    <t>smil1;spol1;spol2;spol3;spol4;smil2;spol5;spol6;smil3/smil4;spol7</t>
+  </si>
+  <si>
+    <t>Chevalier</t>
+  </si>
+  <si>
+    <t>cmil1;cmil2/cmil5;cmil3/cmil6;cmil4/cmil7;cpol1;cpol2;cpol3;cpol4;cpol5;cpol6</t>
+  </si>
+  <si>
+    <t>spol1;spol3;spol4;smil2;spol6;smil3</t>
+  </si>
+  <si>
+    <t>spol1;spol2;spol4;smil2;spol5;spol6;smil3;spol7</t>
+  </si>
+  <si>
+    <t>spol6;smil4</t>
+  </si>
+  <si>
+    <t>spol3;spol4;spol5;smil3</t>
+  </si>
+  <si>
+    <t>spol1;spol3;spol4;smil2;spol5;spol6;smil3;spol7</t>
+  </si>
+  <si>
+    <t>spol4;smil2;spol5;smil3</t>
+  </si>
+  <si>
+    <t>smil2;cpol6</t>
+  </si>
+  <si>
+    <t>spol4;spol6;smil3</t>
+  </si>
+  <si>
+    <t>spol1;spol4;smil2;spol5</t>
+  </si>
+  <si>
+    <t>spol1;spol4;spol5;spol6;smil3</t>
+  </si>
+  <si>
+    <t>spol4;smil2;spol5;spol6;smil3;smil4</t>
+  </si>
+  <si>
+    <t>cpol1;cpol4;cpol5;cpol6;smil2;spol6;smil3</t>
+  </si>
+  <si>
+    <t>spol1;smil2;spol6</t>
+  </si>
+  <si>
+    <t>spol1;spol3;spol4;spol5;spol6;smil3</t>
+  </si>
+  <si>
+    <t>cpol1;cpol5</t>
+  </si>
+  <si>
+    <t>spol5;spol6;smil3</t>
+  </si>
+  <si>
+    <t>cpol4;cpol5</t>
+  </si>
+  <si>
+    <t>spol1;spol4;smil2;spol6;smil3</t>
+  </si>
+  <si>
+    <t>cpol1;cpol6;spol4;spol6;smil3</t>
+  </si>
+  <si>
+    <t>spol1;spol3;spol4;spol5;smil3</t>
+  </si>
+  <si>
+    <t>spol5;spol6;smil3;spol7</t>
+  </si>
+  <si>
+    <t>spol4;spol5;spol6;smil3;smil4</t>
+  </si>
+  <si>
+    <t>spol4;smil3</t>
+  </si>
+  <si>
+    <t>spol1;spol3;spol4;smil2;spol6</t>
+  </si>
+  <si>
+    <t>spol4;spol5;smil3</t>
+  </si>
+  <si>
+    <t>cpol1;spol4;spol6;smil3</t>
+  </si>
+  <si>
+    <t>smil2;spol5</t>
+  </si>
+  <si>
+    <t>spol2;spol5;spol6;smil4</t>
+  </si>
+  <si>
+    <t>spol2;smil2;spol5;spol6;smil4</t>
+  </si>
+  <si>
+    <t>spol1;spol3;spol4;smil2;spol5;smil3</t>
+  </si>
+  <si>
+    <t>spol4;smil2;spol6;smil3</t>
+  </si>
+  <si>
+    <t>spol4;smil2</t>
+  </si>
+  <si>
+    <t>cpol1;spol1;spol3;spol4;smil2;spol5;spol6;smil3;smil4</t>
+  </si>
+  <si>
+    <t>cmil3;cpol1;spol1;spol3;spol4;smil3</t>
+  </si>
+  <si>
+    <t>cmil3;spol1;spol2</t>
+  </si>
+  <si>
+    <t>spol3;spol4;smil2</t>
+  </si>
+  <si>
+    <t>cpol4;cpol6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1264,8 +1397,44 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1344,6 +1513,18 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor rgb="FFFBE5D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1375,7 +1556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1411,6 +1592,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8384,4 +8572,587 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="79.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>157</v>
+      </c>
+      <c r="B45" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>165</v>
+      </c>
+      <c r="B48" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>177</v>
+      </c>
+      <c r="B52" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>187</v>
+      </c>
+      <c r="B56" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>196</v>
+      </c>
+      <c r="B60" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>198</v>
+      </c>
+      <c r="B61" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>200</v>
+      </c>
+      <c r="B62" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>203</v>
+      </c>
+      <c r="B63" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>207</v>
+      </c>
+      <c r="B64" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>211</v>
+      </c>
+      <c r="B65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>214</v>
+      </c>
+      <c r="B66" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>218</v>
+      </c>
+      <c r="B68" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>